<commit_message>
Increasing of 1 the I position of Dardanelles
</commit_message>
<xml_diff>
--- a/river_8_on_meshgrid_v2_4.xlsx
+++ b/river_8_on_meshgrid_v2_4.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="160" windowWidth="38180" windowHeight="22840" tabRatio="908" activeTab="6"/>
+    <workbookView xWindow="14760" yWindow="280" windowWidth="25600" windowHeight="14720" tabRatio="908"/>
   </bookViews>
   <sheets>
     <sheet name="monthly" sheetId="1" r:id="rId1"/>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E43"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2352,8 +2352,12 @@
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="C30">
+        <v>141</v>
+      </c>
       <c r="D30">
-        <v>141</v>
+        <f>C30+1</f>
+        <v>142</v>
       </c>
       <c r="E30">
         <v>41</v>
@@ -2414,8 +2418,12 @@
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="C31">
+        <v>141</v>
+      </c>
       <c r="D31">
-        <v>141</v>
+        <f t="shared" ref="D31:D43" si="0">C31+1</f>
+        <v>142</v>
       </c>
       <c r="E31">
         <v>41</v>
@@ -2476,8 +2484,12 @@
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="C32">
+        <v>140</v>
+      </c>
       <c r="D32">
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>141</v>
       </c>
       <c r="E32">
         <v>41</v>
@@ -2538,8 +2550,12 @@
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="C33">
+        <v>140</v>
+      </c>
       <c r="D33">
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>141</v>
       </c>
       <c r="E33">
         <v>41</v>
@@ -2600,8 +2616,12 @@
       <c r="A34">
         <v>33</v>
       </c>
+      <c r="C34">
+        <v>140</v>
+      </c>
       <c r="D34">
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>141</v>
       </c>
       <c r="E34">
         <v>41</v>
@@ -2662,8 +2682,12 @@
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="C35">
+        <v>141</v>
+      </c>
       <c r="D35">
-        <v>141</v>
+        <f t="shared" si="0"/>
+        <v>142</v>
       </c>
       <c r="E35">
         <v>41</v>
@@ -2724,8 +2748,12 @@
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="C36">
+        <v>141</v>
+      </c>
       <c r="D36">
-        <v>141</v>
+        <f t="shared" si="0"/>
+        <v>142</v>
       </c>
       <c r="E36">
         <v>41</v>
@@ -2786,8 +2814,12 @@
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="C37">
+        <v>140</v>
+      </c>
       <c r="D37">
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>141</v>
       </c>
       <c r="E37">
         <v>41</v>
@@ -2848,8 +2880,12 @@
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="C38">
+        <v>140</v>
+      </c>
       <c r="D38">
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>141</v>
       </c>
       <c r="E38">
         <v>41</v>
@@ -2910,8 +2946,12 @@
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="C39">
+        <v>140</v>
+      </c>
       <c r="D39">
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>141</v>
       </c>
       <c r="E39">
         <v>41</v>
@@ -2972,8 +3012,12 @@
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="C40">
+        <v>141</v>
+      </c>
       <c r="D40">
-        <v>141</v>
+        <f t="shared" si="0"/>
+        <v>142</v>
       </c>
       <c r="E40">
         <v>41</v>
@@ -3034,8 +3078,12 @@
       <c r="A41">
         <v>40</v>
       </c>
+      <c r="C41">
+        <v>141</v>
+      </c>
       <c r="D41">
-        <v>141</v>
+        <f t="shared" si="0"/>
+        <v>142</v>
       </c>
       <c r="E41">
         <v>41</v>
@@ -3096,8 +3144,12 @@
       <c r="A42">
         <v>41</v>
       </c>
+      <c r="C42">
+        <v>140</v>
+      </c>
       <c r="D42">
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>141</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -3158,8 +3210,12 @@
       <c r="A43">
         <v>42</v>
       </c>
+      <c r="C43">
+        <v>140</v>
+      </c>
       <c r="D43">
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>141</v>
       </c>
       <c r="E43">
         <v>40</v>
@@ -33770,7 +33826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:I43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Undoing last comment, return to 4179bed838f7aeb94 state
</commit_message>
<xml_diff>
--- a/river_8_on_meshgrid_v2_4.xlsx
+++ b/river_8_on_meshgrid_v2_4.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="280" windowWidth="25600" windowHeight="14720" tabRatio="908"/>
+    <workbookView xWindow="13500" yWindow="160" windowWidth="38180" windowHeight="22840" tabRatio="908" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="monthly" sheetId="1" r:id="rId1"/>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:D43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2352,12 +2352,8 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>141</v>
-      </c>
-      <c r="D30">
-        <f>C30+1</f>
-        <v>142</v>
       </c>
       <c r="E30">
         <v>41</v>
@@ -2418,12 +2414,8 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>141</v>
-      </c>
-      <c r="D31">
-        <f t="shared" ref="D31:D43" si="0">C31+1</f>
-        <v>142</v>
       </c>
       <c r="E31">
         <v>41</v>
@@ -2484,12 +2476,8 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>140</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
-        <v>141</v>
       </c>
       <c r="E32">
         <v>41</v>
@@ -2550,12 +2538,8 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>140</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="0"/>
-        <v>141</v>
       </c>
       <c r="E33">
         <v>41</v>
@@ -2616,12 +2600,8 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>140</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
-        <v>141</v>
       </c>
       <c r="E34">
         <v>41</v>
@@ -2682,12 +2662,8 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>141</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="0"/>
-        <v>142</v>
       </c>
       <c r="E35">
         <v>41</v>
@@ -2748,12 +2724,8 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>141</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="0"/>
-        <v>142</v>
       </c>
       <c r="E36">
         <v>41</v>
@@ -2814,12 +2786,8 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>140</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="0"/>
-        <v>141</v>
       </c>
       <c r="E37">
         <v>41</v>
@@ -2880,12 +2848,8 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>140</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="0"/>
-        <v>141</v>
       </c>
       <c r="E38">
         <v>41</v>
@@ -2946,12 +2910,8 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>140</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="0"/>
-        <v>141</v>
       </c>
       <c r="E39">
         <v>41</v>
@@ -3012,12 +2972,8 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>141</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="0"/>
-        <v>142</v>
       </c>
       <c r="E40">
         <v>41</v>
@@ -3078,12 +3034,8 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>141</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="0"/>
-        <v>142</v>
       </c>
       <c r="E41">
         <v>41</v>
@@ -3144,12 +3096,8 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>140</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="0"/>
-        <v>141</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -3210,12 +3158,8 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>140</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="0"/>
-        <v>141</v>
       </c>
       <c r="E43">
         <v>40</v>
@@ -33826,7 +33770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:I43"/>
     </sheetView>
   </sheetViews>

</xml_diff>